<commit_message>
Added rudimentary data preparation and updated data
</commit_message>
<xml_diff>
--- a/sv/data/test.xlsx
+++ b/sv/data/test.xlsx
@@ -80,64 +80,64 @@
     <t>cost</t>
   </si>
   <si>
-    <t>Alex Albon</t>
+    <t>albon</t>
   </si>
   <si>
-    <t>Charles Lecrlec</t>
+    <t>leclerc</t>
   </si>
   <si>
-    <t>Esteban Ocon</t>
+    <t>ocon</t>
   </si>
   <si>
-    <t>Fernando Alonso</t>
+    <t>alonso</t>
   </si>
   <si>
-    <t>George Russel</t>
+    <t>russel</t>
   </si>
   <si>
-    <t>Guanyu Zhou</t>
+    <t>zhou</t>
   </si>
   <si>
-    <t>Kevin Magnussen</t>
+    <t>magnussen</t>
   </si>
   <si>
-    <t>Lance Stroll</t>
+    <t>stroll</t>
   </si>
   <si>
-    <t>Lando Norris</t>
+    <t>norris</t>
   </si>
   <si>
-    <t>Lewis Hamilton</t>
+    <t>hamilton</t>
   </si>
   <si>
-    <t>Logan Sargeant</t>
+    <t>sargeant</t>
   </si>
   <si>
-    <t>Max Verstappen</t>
+    <t>verstappen</t>
   </si>
   <si>
-    <t>Nico Hulkenberg</t>
+    <t>hulkenberg</t>
   </si>
   <si>
-    <t>Ricardo</t>
+    <t>ricardo</t>
   </si>
   <si>
-    <t>Oscar Piastri</t>
+    <t>piastri</t>
   </si>
   <si>
-    <t>Pierre Gasly</t>
+    <t>gasly</t>
   </si>
   <si>
-    <t>Carlos Sainz</t>
+    <t>sainz</t>
   </si>
   <si>
-    <t>Sergio Perez</t>
+    <t>perez</t>
   </si>
   <si>
-    <t>Valtreri Bottas</t>
+    <t>bottas</t>
   </si>
   <si>
-    <t>Yuki Tsunoda</t>
+    <t>tsunoda</t>
   </si>
   <si>
     <t>Alfa Romeo</t>
@@ -536,6 +536,9 @@
         <v>8.0</v>
       </c>
       <c r="S2" s="2"/>
+      <c r="W2" s="1">
+        <v>6.9</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="s">
@@ -575,6 +578,9 @@
         <v>6.0</v>
       </c>
       <c r="S3" s="2"/>
+      <c r="W3" s="1">
+        <v>21.9</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="s">
@@ -614,6 +620,9 @@
         <v>-18.0</v>
       </c>
       <c r="S4" s="2"/>
+      <c r="W4" s="1">
+        <v>9.8</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="s">
@@ -653,6 +662,9 @@
         <v>12.0</v>
       </c>
       <c r="S5" s="2"/>
+      <c r="W5" s="1">
+        <v>11.4</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="s">
@@ -692,6 +704,9 @@
         <v>18.0</v>
       </c>
       <c r="S6" s="2"/>
+      <c r="W6" s="1">
+        <v>18.8</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="s">
@@ -731,6 +746,9 @@
         <v>6.0</v>
       </c>
       <c r="S7" s="2"/>
+      <c r="W7" s="1">
+        <v>5.2</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="s">
@@ -770,6 +788,9 @@
         <v>-19.0</v>
       </c>
       <c r="S8" s="2"/>
+      <c r="W8" s="1">
+        <v>6.8</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="s">
@@ -809,6 +830,9 @@
         <v>2.0</v>
       </c>
       <c r="S9" s="2"/>
+      <c r="W9" s="1">
+        <v>8.6</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="s">
@@ -848,6 +872,9 @@
         <v>38.0</v>
       </c>
       <c r="S10" s="2"/>
+      <c r="W10" s="1">
+        <v>12.9</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="s">
@@ -887,6 +914,9 @@
         <v>25.0</v>
       </c>
       <c r="S11" s="2"/>
+      <c r="W11" s="1">
+        <v>24.7</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12" s="1" t="s">
@@ -926,6 +956,9 @@
         <v>6.0</v>
       </c>
       <c r="S12" s="2"/>
+      <c r="W12" s="1">
+        <v>4.5</v>
+      </c>
     </row>
     <row r="13">
       <c r="A13" s="1" t="s">
@@ -965,6 +998,9 @@
         <v>46.0</v>
       </c>
       <c r="S13" s="2"/>
+      <c r="W13" s="1">
+        <v>28.1</v>
+      </c>
     </row>
     <row r="14">
       <c r="A14" s="1" t="s">
@@ -1004,6 +1040,9 @@
         <v>0.0</v>
       </c>
       <c r="S14" s="2"/>
+      <c r="W14" s="1">
+        <v>3.8</v>
+      </c>
     </row>
     <row r="15">
       <c r="A15" s="1" t="s">
@@ -1043,6 +1082,9 @@
         <v>0.0</v>
       </c>
       <c r="S15" s="2"/>
+      <c r="W15" s="1">
+        <v>4.5</v>
+      </c>
     </row>
     <row r="16">
       <c r="A16" s="1" t="s">
@@ -1082,6 +1124,9 @@
         <v>20.0</v>
       </c>
       <c r="S16" s="2"/>
+      <c r="W16" s="1">
+        <v>8.0</v>
+      </c>
     </row>
     <row r="17">
       <c r="A17" s="1" t="s">
@@ -1121,6 +1166,9 @@
         <v>-3.0</v>
       </c>
       <c r="S17" s="2"/>
+      <c r="W17" s="1">
+        <v>8.6</v>
+      </c>
     </row>
     <row r="18">
       <c r="A18" s="1" t="s">
@@ -1160,6 +1208,9 @@
         <v>4.0</v>
       </c>
       <c r="S18" s="2"/>
+      <c r="W18" s="1">
+        <v>17.4</v>
+      </c>
     </row>
     <row r="19">
       <c r="A19" s="1" t="s">
@@ -1199,6 +1250,9 @@
         <v>26.0</v>
       </c>
       <c r="S19" s="2"/>
+      <c r="W19" s="1">
+        <v>19.3</v>
+      </c>
     </row>
     <row r="20">
       <c r="A20" s="1" t="s">
@@ -1238,6 +1292,9 @@
         <v>-5.0</v>
       </c>
       <c r="S20" s="2"/>
+      <c r="W20" s="1">
+        <v>7.9</v>
+      </c>
     </row>
     <row r="21">
       <c r="A21" s="1" t="s">
@@ -1277,6 +1334,9 @@
         <v>3.0</v>
       </c>
       <c r="S21" s="2"/>
+      <c r="W21" s="1">
+        <v>5.1</v>
+      </c>
     </row>
     <row r="22">
       <c r="S22" s="2"/>

</xml_diff>

<commit_message>
Updated dataset, optimization now works
</commit_message>
<xml_diff>
--- a/sv/data/test.xlsx
+++ b/sv/data/test.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="52">
   <si>
     <t>r0</t>
   </si>
@@ -201,7 +201,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -209,7 +209,6 @@
       <alignment readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="2" xfId="0" applyFont="1" applyNumberFormat="1"/>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle xfId="0" name="Normal" builtinId="0"/>
@@ -535,9 +534,12 @@
       <c r="L2" s="1">
         <v>8.0</v>
       </c>
+      <c r="M2" s="1">
+        <v>8.0</v>
+      </c>
       <c r="S2" s="2"/>
       <c r="W2" s="1">
-        <v>6.9</v>
+        <v>7.4</v>
       </c>
     </row>
     <row r="3">
@@ -577,9 +579,12 @@
       <c r="L3" s="1">
         <v>6.0</v>
       </c>
+      <c r="M3" s="1">
+        <v>12.0</v>
+      </c>
       <c r="S3" s="2"/>
       <c r="W3" s="1">
-        <v>21.9</v>
+        <v>22.0</v>
       </c>
     </row>
     <row r="4">
@@ -619,9 +624,12 @@
       <c r="L4" s="1">
         <v>-18.0</v>
       </c>
+      <c r="M4" s="1">
+        <v>-19.0</v>
+      </c>
       <c r="S4" s="2"/>
       <c r="W4" s="1">
-        <v>9.8</v>
+        <v>9.7</v>
       </c>
     </row>
     <row r="5">
@@ -661,9 +669,12 @@
       <c r="L5" s="1">
         <v>12.0</v>
       </c>
+      <c r="M5" s="1">
+        <v>7.0</v>
+      </c>
       <c r="S5" s="2"/>
       <c r="W5" s="1">
-        <v>11.4</v>
+        <v>11.9</v>
       </c>
     </row>
     <row r="6">
@@ -703,9 +714,12 @@
       <c r="L6" s="1">
         <v>18.0</v>
       </c>
+      <c r="M6" s="1">
+        <v>27.0</v>
+      </c>
       <c r="S6" s="2"/>
       <c r="W6" s="1">
-        <v>18.8</v>
+        <v>19.1</v>
       </c>
     </row>
     <row r="7">
@@ -745,6 +759,9 @@
       <c r="L7" s="1">
         <v>6.0</v>
       </c>
+      <c r="M7" s="1">
+        <v>-4.0</v>
+      </c>
       <c r="S7" s="2"/>
       <c r="W7" s="1">
         <v>5.2</v>
@@ -787,6 +804,9 @@
       <c r="L8" s="1">
         <v>-19.0</v>
       </c>
+      <c r="M8" s="1">
+        <v>5.0</v>
+      </c>
       <c r="S8" s="2"/>
       <c r="W8" s="1">
         <v>6.8</v>
@@ -829,9 +849,12 @@
       <c r="L9" s="1">
         <v>2.0</v>
       </c>
+      <c r="M9" s="1">
+        <v>9.0</v>
+      </c>
       <c r="S9" s="2"/>
       <c r="W9" s="1">
-        <v>8.6</v>
+        <v>9.1</v>
       </c>
     </row>
     <row r="10">
@@ -871,9 +894,12 @@
       <c r="L10" s="1">
         <v>38.0</v>
       </c>
+      <c r="M10" s="1">
+        <v>29.0</v>
+      </c>
       <c r="S10" s="2"/>
       <c r="W10" s="1">
-        <v>12.9</v>
+        <v>13.9</v>
       </c>
     </row>
     <row r="11">
@@ -913,9 +939,12 @@
       <c r="L11" s="1">
         <v>25.0</v>
       </c>
+      <c r="M11" s="1">
+        <v>20.0</v>
+      </c>
       <c r="S11" s="2"/>
       <c r="W11" s="1">
-        <v>24.7</v>
+        <v>25.0</v>
       </c>
     </row>
     <row r="12">
@@ -955,6 +984,9 @@
       <c r="L12" s="1">
         <v>6.0</v>
       </c>
+      <c r="M12" s="1">
+        <v>2.0</v>
+      </c>
       <c r="S12" s="2"/>
       <c r="W12" s="1">
         <v>4.5</v>
@@ -997,9 +1029,12 @@
       <c r="L13" s="1">
         <v>46.0</v>
       </c>
+      <c r="M13" s="1">
+        <v>46.0</v>
+      </c>
       <c r="S13" s="2"/>
       <c r="W13" s="1">
-        <v>28.1</v>
+        <v>28.3</v>
       </c>
     </row>
     <row r="14">
@@ -1039,6 +1074,9 @@
       <c r="L14" s="1">
         <v>0.0</v>
       </c>
+      <c r="M14" s="1">
+        <v>0.0</v>
+      </c>
       <c r="S14" s="2"/>
       <c r="W14" s="1">
         <v>3.8</v>
@@ -1081,6 +1119,9 @@
       <c r="L15" s="1">
         <v>0.0</v>
       </c>
+      <c r="M15" s="1">
+        <v>2.0</v>
+      </c>
       <c r="S15" s="2"/>
       <c r="W15" s="1">
         <v>4.5</v>
@@ -1123,9 +1164,12 @@
       <c r="L16" s="1">
         <v>20.0</v>
       </c>
+      <c r="M16" s="1">
+        <v>18.0</v>
+      </c>
       <c r="S16" s="2"/>
       <c r="W16" s="1">
-        <v>8.0</v>
+        <v>9.0</v>
       </c>
     </row>
     <row r="17">
@@ -1165,9 +1209,12 @@
       <c r="L17" s="1">
         <v>-3.0</v>
       </c>
+      <c r="M17" s="1">
+        <v>-19.0</v>
+      </c>
       <c r="S17" s="2"/>
       <c r="W17" s="1">
-        <v>8.6</v>
+        <v>8.5</v>
       </c>
     </row>
     <row r="18">
@@ -1207,9 +1254,12 @@
       <c r="L18" s="1">
         <v>4.0</v>
       </c>
+      <c r="M18" s="1">
+        <v>12.0</v>
+      </c>
       <c r="S18" s="2"/>
       <c r="W18" s="1">
-        <v>17.4</v>
+        <v>17.5</v>
       </c>
     </row>
     <row r="19">
@@ -1249,9 +1299,12 @@
       <c r="L19" s="1">
         <v>26.0</v>
       </c>
+      <c r="M19" s="1">
+        <v>39.0</v>
+      </c>
       <c r="S19" s="2"/>
       <c r="W19" s="1">
-        <v>19.3</v>
+        <v>20.3</v>
       </c>
     </row>
     <row r="20">
@@ -1291,6 +1344,9 @@
       <c r="L20" s="1">
         <v>-5.0</v>
       </c>
+      <c r="M20" s="1">
+        <v>0.0</v>
+      </c>
       <c r="S20" s="2"/>
       <c r="W20" s="1">
         <v>7.9</v>
@@ -1332,6 +1388,9 @@
       </c>
       <c r="L21" s="1">
         <v>3.0</v>
+      </c>
+      <c r="M21" s="1">
+        <v>5.0</v>
       </c>
       <c r="S21" s="2"/>
       <c r="W21" s="1">
@@ -4291,578 +4350,532 @@
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="B1" s="1">
-        <v>31.0</v>
-      </c>
-      <c r="C1" s="1">
-        <v>7.0</v>
-      </c>
-      <c r="D1" s="1">
-        <v>26.0</v>
-      </c>
-      <c r="E1" s="1">
-        <v>-10.0</v>
-      </c>
-      <c r="F1" s="1">
-        <v>8.0</v>
-      </c>
-      <c r="G1" s="1">
-        <v>0.0</v>
-      </c>
-      <c r="H1" s="1">
-        <v>22.0</v>
-      </c>
-      <c r="I1" s="1">
-        <v>19.0</v>
-      </c>
-      <c r="J1" s="1">
-        <v>11.0</v>
-      </c>
-      <c r="K1" s="1">
-        <v>16.0</v>
-      </c>
-      <c r="L1" s="1">
-        <v>0.0</v>
-      </c>
-      <c r="O1" s="3">
-        <f t="shared" ref="O1:O10" si="1">SUM(B1:L1)</f>
-        <v>130</v>
-      </c>
-      <c r="P1" s="3">
-        <f t="shared" ref="P1:P10" si="2">SUM(H1:L1)</f>
-        <v>68</v>
-      </c>
-      <c r="T1" s="2">
-        <f t="shared" ref="T1:T10" si="3">O1/X1</f>
-        <v>22.03389831</v>
-      </c>
-      <c r="V1" s="2">
-        <f t="shared" ref="V1:V10" si="4">P1/X1</f>
-        <v>11.52542373</v>
-      </c>
-      <c r="X1" s="1">
-        <v>5.9</v>
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="T1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="U1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="V1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="W1" s="1" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B2" s="1">
-        <v>17.0</v>
+        <v>31.0</v>
       </c>
       <c r="C2" s="1">
-        <v>15.0</v>
+        <v>7.0</v>
       </c>
       <c r="D2" s="1">
-        <v>13.0</v>
+        <v>26.0</v>
       </c>
       <c r="E2" s="1">
-        <v>-23.0</v>
+        <v>-10.0</v>
       </c>
       <c r="F2" s="1">
-        <v>17.0</v>
+        <v>8.0</v>
       </c>
       <c r="G2" s="1">
         <v>0.0</v>
       </c>
       <c r="H2" s="1">
-        <v>1.0</v>
+        <v>22.0</v>
       </c>
       <c r="I2" s="1">
-        <v>20.0</v>
+        <v>19.0</v>
       </c>
       <c r="J2" s="1">
+        <v>11.0</v>
+      </c>
+      <c r="K2" s="1">
+        <v>16.0</v>
+      </c>
+      <c r="L2" s="1">
+        <v>0.0</v>
+      </c>
+      <c r="M2" s="1">
         <v>6.0</v>
       </c>
-      <c r="K2" s="1">
-        <v>20.0</v>
-      </c>
-      <c r="L2" s="1">
-        <v>5.0</v>
-      </c>
-      <c r="O2" s="3">
-        <f t="shared" si="1"/>
-        <v>91</v>
-      </c>
-      <c r="P2" s="3">
-        <f t="shared" si="2"/>
-        <v>52</v>
-      </c>
-      <c r="T2" s="2">
-        <f t="shared" si="3"/>
-        <v>15.16666667</v>
-      </c>
-      <c r="V2" s="2">
-        <f t="shared" si="4"/>
-        <v>8.666666667</v>
-      </c>
-      <c r="X2" s="1">
-        <v>6.0</v>
+      <c r="T2" s="2"/>
+      <c r="V2" s="2"/>
+      <c r="W2" s="1">
+        <v>5.9</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B3" s="1">
-        <v>8.0</v>
+        <v>17.0</v>
       </c>
       <c r="C3" s="1">
-        <v>28.0</v>
+        <v>15.0</v>
       </c>
       <c r="D3" s="1">
-        <v>11.0</v>
+        <v>13.0</v>
       </c>
       <c r="E3" s="1">
-        <v>25.0</v>
+        <v>-23.0</v>
       </c>
       <c r="F3" s="1">
-        <v>28.0</v>
+        <v>17.0</v>
       </c>
       <c r="G3" s="1">
         <v>0.0</v>
       </c>
       <c r="H3" s="1">
-        <v>42.0</v>
+        <v>1.0</v>
       </c>
       <c r="I3" s="1">
-        <v>33.0</v>
+        <v>20.0</v>
       </c>
       <c r="J3" s="1">
-        <v>24.0</v>
+        <v>6.0</v>
       </c>
       <c r="K3" s="1">
-        <v>21.0</v>
+        <v>20.0</v>
       </c>
       <c r="L3" s="1">
-        <v>-16.0</v>
-      </c>
-      <c r="O3" s="3">
-        <f t="shared" si="1"/>
-        <v>204</v>
-      </c>
-      <c r="P3" s="3">
-        <f t="shared" si="2"/>
-        <v>104</v>
-      </c>
-      <c r="T3" s="2">
-        <f t="shared" si="3"/>
-        <v>19.61538462</v>
-      </c>
-      <c r="V3" s="2">
-        <f t="shared" si="4"/>
-        <v>10</v>
-      </c>
-      <c r="X3" s="1">
-        <v>10.4</v>
+        <v>5.0</v>
+      </c>
+      <c r="M3" s="1">
+        <v>8.0</v>
+      </c>
+      <c r="T3" s="2"/>
+      <c r="V3" s="2"/>
+      <c r="W3" s="1">
+        <v>6.0</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B4" s="1">
-        <v>56.0</v>
+        <v>8.0</v>
       </c>
       <c r="C4" s="1">
-        <v>19.0</v>
+        <v>28.0</v>
       </c>
       <c r="D4" s="1">
-        <v>54.0</v>
+        <v>11.0</v>
       </c>
       <c r="E4" s="1">
-        <v>55.0</v>
+        <v>25.0</v>
       </c>
       <c r="F4" s="1">
-        <v>42.0</v>
+        <v>28.0</v>
       </c>
       <c r="G4" s="1">
         <v>0.0</v>
       </c>
       <c r="H4" s="1">
-        <v>15.0</v>
+        <v>42.0</v>
       </c>
       <c r="I4" s="1">
-        <v>40.0</v>
+        <v>33.0</v>
       </c>
       <c r="J4" s="1">
-        <v>46.0</v>
+        <v>24.0</v>
       </c>
       <c r="K4" s="1">
-        <v>63.0</v>
+        <v>21.0</v>
       </c>
       <c r="L4" s="1">
-        <v>22.0</v>
-      </c>
-      <c r="O4" s="3">
-        <f t="shared" si="1"/>
-        <v>412</v>
-      </c>
-      <c r="P4" s="3">
-        <f t="shared" si="2"/>
-        <v>186</v>
-      </c>
-      <c r="T4" s="2">
-        <f t="shared" si="3"/>
-        <v>45.77777778</v>
-      </c>
-      <c r="V4" s="2">
-        <f t="shared" si="4"/>
-        <v>20.66666667</v>
-      </c>
-      <c r="X4" s="1">
-        <v>9.0</v>
+        <v>-16.0</v>
+      </c>
+      <c r="M4" s="1">
+        <v>-35.0</v>
+      </c>
+      <c r="T4" s="2"/>
+      <c r="V4" s="2"/>
+      <c r="W4" s="1">
+        <v>10.3</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B5" s="1">
-        <v>31.0</v>
+        <v>56.0</v>
       </c>
       <c r="C5" s="1">
-        <v>59.0</v>
+        <v>19.0</v>
       </c>
       <c r="D5" s="1">
-        <v>3.0</v>
+        <v>54.0</v>
       </c>
       <c r="E5" s="1">
-        <v>63.0</v>
+        <v>55.0</v>
       </c>
       <c r="F5" s="1">
-        <v>56.0</v>
+        <v>42.0</v>
       </c>
       <c r="G5" s="1">
         <v>0.0</v>
       </c>
       <c r="H5" s="1">
-        <v>37.0</v>
+        <v>15.0</v>
       </c>
       <c r="I5" s="1">
-        <v>38.0</v>
+        <v>40.0</v>
       </c>
       <c r="J5" s="1">
         <v>46.0</v>
       </c>
       <c r="K5" s="1">
-        <v>73.0</v>
+        <v>63.0</v>
       </c>
       <c r="L5" s="1">
-        <v>25.0</v>
-      </c>
-      <c r="O5" s="3">
-        <f t="shared" si="1"/>
-        <v>431</v>
-      </c>
-      <c r="P5" s="3">
-        <f t="shared" si="2"/>
-        <v>219</v>
-      </c>
-      <c r="T5" s="2">
-        <f t="shared" si="3"/>
-        <v>18.8209607</v>
-      </c>
-      <c r="V5" s="2">
-        <f t="shared" si="4"/>
-        <v>9.563318777</v>
-      </c>
-      <c r="X5" s="1">
-        <v>22.9</v>
+        <v>22.0</v>
+      </c>
+      <c r="M5" s="1">
+        <v>21.0</v>
+      </c>
+      <c r="T5" s="2"/>
+      <c r="V5" s="2"/>
+      <c r="W5" s="1">
+        <v>9.5</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B6" s="1">
-        <v>12.0</v>
+        <v>31.0</v>
       </c>
       <c r="C6" s="1">
-        <v>13.0</v>
+        <v>59.0</v>
       </c>
       <c r="D6" s="1">
-        <v>18.0</v>
+        <v>3.0</v>
       </c>
       <c r="E6" s="1">
-        <v>17.0</v>
+        <v>63.0</v>
       </c>
       <c r="F6" s="1">
-        <v>15.0</v>
+        <v>56.0</v>
       </c>
       <c r="G6" s="1">
         <v>0.0</v>
       </c>
       <c r="H6" s="1">
-        <v>7.0</v>
+        <v>37.0</v>
       </c>
       <c r="I6" s="1">
-        <v>17.0</v>
+        <v>38.0</v>
       </c>
       <c r="J6" s="1">
-        <v>4.0</v>
+        <v>46.0</v>
       </c>
       <c r="K6" s="1">
-        <v>14.0</v>
+        <v>73.0</v>
       </c>
       <c r="L6" s="1">
-        <v>-18.0</v>
-      </c>
-      <c r="O6" s="3">
-        <f t="shared" si="1"/>
-        <v>99</v>
-      </c>
-      <c r="P6" s="3">
-        <f t="shared" si="2"/>
-        <v>24</v>
-      </c>
-      <c r="T6" s="2">
-        <f t="shared" si="3"/>
-        <v>20.20408163</v>
-      </c>
-      <c r="V6" s="2">
-        <f t="shared" si="4"/>
-        <v>4.897959184</v>
-      </c>
-      <c r="X6" s="1">
-        <v>4.9</v>
+        <v>25.0</v>
+      </c>
+      <c r="M6" s="1">
+        <v>32.0</v>
+      </c>
+      <c r="T6" s="2"/>
+      <c r="V6" s="2"/>
+      <c r="W6" s="1">
+        <v>23.0</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B7" s="1">
-        <v>-16.0</v>
+        <v>12.0</v>
       </c>
       <c r="C7" s="1">
-        <v>14.0</v>
+        <v>13.0</v>
       </c>
       <c r="D7" s="1">
-        <v>36.0</v>
+        <v>18.0</v>
       </c>
       <c r="E7" s="1">
-        <v>23.0</v>
+        <v>17.0</v>
       </c>
       <c r="F7" s="1">
-        <v>8.0</v>
+        <v>15.0</v>
       </c>
       <c r="G7" s="1">
         <v>0.0</v>
       </c>
       <c r="H7" s="1">
-        <v>15.0</v>
+        <v>7.0</v>
       </c>
       <c r="I7" s="1">
-        <v>11.0</v>
+        <v>17.0</v>
       </c>
       <c r="J7" s="1">
-        <v>15.0</v>
+        <v>4.0</v>
       </c>
       <c r="K7" s="1">
-        <v>54.0</v>
+        <v>14.0</v>
       </c>
       <c r="L7" s="1">
-        <v>68.0</v>
-      </c>
-      <c r="O7" s="3">
-        <f t="shared" si="1"/>
-        <v>228</v>
-      </c>
-      <c r="P7" s="3">
-        <f t="shared" si="2"/>
-        <v>163</v>
-      </c>
-      <c r="T7" s="2">
-        <f t="shared" si="3"/>
-        <v>21.11111111</v>
-      </c>
-      <c r="V7" s="2">
-        <f t="shared" si="4"/>
-        <v>15.09259259</v>
-      </c>
-      <c r="X7" s="1">
-        <v>10.8</v>
+        <v>-18.0</v>
+      </c>
+      <c r="M7" s="1">
+        <v>10.0</v>
+      </c>
+      <c r="T7" s="2"/>
+      <c r="V7" s="2"/>
+      <c r="W7" s="1">
+        <v>4.9</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B8" s="1">
-        <v>45.0</v>
+        <v>-16.0</v>
       </c>
       <c r="C8" s="1">
-        <v>44.0</v>
+        <v>14.0</v>
       </c>
       <c r="D8" s="1">
-        <v>32.0</v>
+        <v>36.0</v>
       </c>
       <c r="E8" s="1">
-        <v>49.0</v>
+        <v>23.0</v>
       </c>
       <c r="F8" s="1">
-        <v>57.0</v>
+        <v>8.0</v>
       </c>
       <c r="G8" s="1">
         <v>0.0</v>
       </c>
       <c r="H8" s="1">
+        <v>15.0</v>
+      </c>
+      <c r="I8" s="1">
+        <v>11.0</v>
+      </c>
+      <c r="J8" s="1">
+        <v>15.0</v>
+      </c>
+      <c r="K8" s="1">
         <v>54.0</v>
       </c>
-      <c r="I8" s="1">
-        <v>65.0</v>
-      </c>
-      <c r="J8" s="1">
-        <v>21.0</v>
-      </c>
-      <c r="K8" s="1">
-        <v>70.0</v>
-      </c>
       <c r="L8" s="1">
-        <v>53.0</v>
-      </c>
-      <c r="O8" s="3">
-        <f t="shared" si="1"/>
-        <v>490</v>
-      </c>
-      <c r="P8" s="3">
-        <f t="shared" si="2"/>
-        <v>263</v>
-      </c>
-      <c r="T8" s="2">
-        <f t="shared" si="3"/>
-        <v>19.36758893</v>
-      </c>
-      <c r="V8" s="2">
-        <f t="shared" si="4"/>
-        <v>10.39525692</v>
-      </c>
-      <c r="X8" s="1">
-        <v>25.3</v>
+        <v>68.0</v>
+      </c>
+      <c r="M8" s="1">
+        <v>62.0</v>
+      </c>
+      <c r="T8" s="2"/>
+      <c r="V8" s="2"/>
+      <c r="W8" s="1">
+        <v>11.8</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B9" s="1">
-        <v>78.0</v>
+        <v>45.0</v>
       </c>
       <c r="C9" s="1">
-        <v>95.0</v>
+        <v>44.0</v>
       </c>
       <c r="D9" s="1">
-        <v>98.0</v>
+        <v>32.0</v>
       </c>
       <c r="E9" s="1">
-        <v>108.0</v>
+        <v>49.0</v>
       </c>
       <c r="F9" s="1">
-        <v>97.0</v>
+        <v>57.0</v>
       </c>
       <c r="G9" s="1">
         <v>0.0</v>
       </c>
       <c r="H9" s="1">
-        <v>63.0</v>
+        <v>54.0</v>
       </c>
       <c r="I9" s="1">
-        <v>96.0</v>
+        <v>65.0</v>
       </c>
       <c r="J9" s="1">
-        <v>86.0</v>
+        <v>21.0</v>
       </c>
       <c r="K9" s="1">
-        <v>112.0</v>
+        <v>70.0</v>
       </c>
       <c r="L9" s="1">
-        <v>77.0</v>
-      </c>
-      <c r="O9" s="3">
-        <f t="shared" si="1"/>
-        <v>910</v>
-      </c>
-      <c r="P9" s="3">
-        <f t="shared" si="2"/>
-        <v>434</v>
-      </c>
-      <c r="T9" s="2">
-        <f t="shared" si="3"/>
-        <v>32.04225352</v>
-      </c>
-      <c r="V9" s="2">
-        <f t="shared" si="4"/>
-        <v>15.28169014</v>
-      </c>
-      <c r="X9" s="1">
-        <v>28.4</v>
+        <v>53.0</v>
+      </c>
+      <c r="M9" s="1">
+        <v>52.0</v>
+      </c>
+      <c r="T9" s="2"/>
+      <c r="V9" s="2"/>
+      <c r="W9" s="1">
+        <v>25.4</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B10" s="1">
-        <v>25.0</v>
+        <v>78.0</v>
       </c>
       <c r="C10" s="1">
-        <v>-16.0</v>
+        <v>95.0</v>
       </c>
       <c r="D10" s="1">
-        <v>-5.0</v>
+        <v>98.0</v>
       </c>
       <c r="E10" s="1">
-        <v>-15.0</v>
+        <v>108.0</v>
       </c>
       <c r="F10" s="1">
-        <v>1.0</v>
+        <v>97.0</v>
       </c>
       <c r="G10" s="1">
         <v>0.0</v>
       </c>
       <c r="H10" s="1">
+        <v>63.0</v>
+      </c>
+      <c r="I10" s="1">
+        <v>96.0</v>
+      </c>
+      <c r="J10" s="1">
+        <v>86.0</v>
+      </c>
+      <c r="K10" s="1">
+        <v>112.0</v>
+      </c>
+      <c r="L10" s="1">
+        <v>77.0</v>
+      </c>
+      <c r="M10" s="1">
+        <v>95.0</v>
+      </c>
+      <c r="T10" s="2"/>
+      <c r="V10" s="2"/>
+      <c r="W10" s="1">
+        <v>28.6</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="B11" s="1">
+        <v>25.0</v>
+      </c>
+      <c r="C11" s="1">
+        <v>-16.0</v>
+      </c>
+      <c r="D11" s="1">
+        <v>-5.0</v>
+      </c>
+      <c r="E11" s="1">
+        <v>-15.0</v>
+      </c>
+      <c r="F11" s="1">
         <v>1.0</v>
       </c>
-      <c r="I10" s="1">
+      <c r="G11" s="1">
+        <v>0.0</v>
+      </c>
+      <c r="H11" s="1">
+        <v>1.0</v>
+      </c>
+      <c r="I11" s="1">
         <v>5.0</v>
       </c>
-      <c r="J10" s="1">
+      <c r="J11" s="1">
         <v>-2.0</v>
       </c>
-      <c r="K10" s="1">
+      <c r="K11" s="1">
         <v>35.0</v>
       </c>
-      <c r="L10" s="1">
+      <c r="L11" s="1">
         <v>19.0</v>
       </c>
-      <c r="O10" s="3">
-        <f t="shared" si="1"/>
-        <v>48</v>
-      </c>
-      <c r="P10" s="3">
-        <f t="shared" si="2"/>
-        <v>58</v>
-      </c>
-      <c r="T10" s="2">
-        <f t="shared" si="3"/>
-        <v>8.727272727</v>
-      </c>
-      <c r="V10" s="2">
-        <f t="shared" si="4"/>
-        <v>10.54545455</v>
-      </c>
-      <c r="X10" s="1">
-        <v>5.5</v>
-      </c>
-    </row>
-    <row r="11">
+      <c r="M11" s="1">
+        <v>9.0</v>
+      </c>
       <c r="T11" s="2"/>
       <c r="V11" s="2"/>
+      <c r="W11" s="1">
+        <v>5.5</v>
+      </c>
     </row>
     <row r="12">
       <c r="T12" s="2"/>

</xml_diff>

<commit_message>
Added casting to int
</commit_message>
<xml_diff>
--- a/sv/data/test.xlsx
+++ b/sv/data/test.xlsx
@@ -539,7 +539,7 @@
       </c>
       <c r="S2" s="2"/>
       <c r="W2" s="1">
-        <v>7.4</v>
+        <v>6.9</v>
       </c>
     </row>
     <row r="3">
@@ -584,7 +584,7 @@
       </c>
       <c r="S3" s="2"/>
       <c r="W3" s="1">
-        <v>22.0</v>
+        <v>21.9</v>
       </c>
     </row>
     <row r="4">
@@ -629,7 +629,7 @@
       </c>
       <c r="S4" s="2"/>
       <c r="W4" s="1">
-        <v>9.7</v>
+        <v>9.8</v>
       </c>
     </row>
     <row r="5">
@@ -674,7 +674,7 @@
       </c>
       <c r="S5" s="2"/>
       <c r="W5" s="1">
-        <v>11.9</v>
+        <v>11.4</v>
       </c>
     </row>
     <row r="6">
@@ -719,7 +719,7 @@
       </c>
       <c r="S6" s="2"/>
       <c r="W6" s="1">
-        <v>19.1</v>
+        <v>18.8</v>
       </c>
     </row>
     <row r="7">
@@ -854,7 +854,7 @@
       </c>
       <c r="S9" s="2"/>
       <c r="W9" s="1">
-        <v>9.1</v>
+        <v>8.6</v>
       </c>
     </row>
     <row r="10">
@@ -899,7 +899,7 @@
       </c>
       <c r="S10" s="2"/>
       <c r="W10" s="1">
-        <v>13.9</v>
+        <v>12.9</v>
       </c>
     </row>
     <row r="11">
@@ -944,7 +944,7 @@
       </c>
       <c r="S11" s="2"/>
       <c r="W11" s="1">
-        <v>25.0</v>
+        <v>24.7</v>
       </c>
     </row>
     <row r="12">
@@ -1034,7 +1034,7 @@
       </c>
       <c r="S13" s="2"/>
       <c r="W13" s="1">
-        <v>28.3</v>
+        <v>28.1</v>
       </c>
     </row>
     <row r="14">
@@ -1169,7 +1169,7 @@
       </c>
       <c r="S16" s="2"/>
       <c r="W16" s="1">
-        <v>9.0</v>
+        <v>8.0</v>
       </c>
     </row>
     <row r="17">
@@ -1214,7 +1214,7 @@
       </c>
       <c r="S17" s="2"/>
       <c r="W17" s="1">
-        <v>8.5</v>
+        <v>8.6</v>
       </c>
     </row>
     <row r="18">
@@ -1259,7 +1259,7 @@
       </c>
       <c r="S18" s="2"/>
       <c r="W18" s="1">
-        <v>17.5</v>
+        <v>17.4</v>
       </c>
     </row>
     <row r="19">
@@ -1304,7 +1304,7 @@
       </c>
       <c r="S19" s="2"/>
       <c r="W19" s="1">
-        <v>20.3</v>
+        <v>19.3</v>
       </c>
     </row>
     <row r="20">
@@ -4454,9 +4454,6 @@
       <c r="L2" s="1">
         <v>0.0</v>
       </c>
-      <c r="M2" s="1">
-        <v>6.0</v>
-      </c>
       <c r="T2" s="2"/>
       <c r="V2" s="2"/>
       <c r="W2" s="1">
@@ -4500,9 +4497,6 @@
       <c r="L3" s="1">
         <v>5.0</v>
       </c>
-      <c r="M3" s="1">
-        <v>8.0</v>
-      </c>
       <c r="T3" s="2"/>
       <c r="V3" s="2"/>
       <c r="W3" s="1">
@@ -4546,13 +4540,10 @@
       <c r="L4" s="1">
         <v>-16.0</v>
       </c>
-      <c r="M4" s="1">
-        <v>-35.0</v>
-      </c>
       <c r="T4" s="2"/>
       <c r="V4" s="2"/>
       <c r="W4" s="1">
-        <v>10.3</v>
+        <v>10.4</v>
       </c>
     </row>
     <row r="5">
@@ -4592,13 +4583,10 @@
       <c r="L5" s="1">
         <v>22.0</v>
       </c>
-      <c r="M5" s="1">
-        <v>21.0</v>
-      </c>
       <c r="T5" s="2"/>
       <c r="V5" s="2"/>
       <c r="W5" s="1">
-        <v>9.5</v>
+        <v>9.0</v>
       </c>
     </row>
     <row r="6">
@@ -4638,13 +4626,10 @@
       <c r="L6" s="1">
         <v>25.0</v>
       </c>
-      <c r="M6" s="1">
-        <v>32.0</v>
-      </c>
       <c r="T6" s="2"/>
       <c r="V6" s="2"/>
       <c r="W6" s="1">
-        <v>23.0</v>
+        <v>29.9</v>
       </c>
     </row>
     <row r="7">
@@ -4683,9 +4668,6 @@
       </c>
       <c r="L7" s="1">
         <v>-18.0</v>
-      </c>
-      <c r="M7" s="1">
-        <v>10.0</v>
       </c>
       <c r="T7" s="2"/>
       <c r="V7" s="2"/>
@@ -4730,13 +4712,10 @@
       <c r="L8" s="1">
         <v>68.0</v>
       </c>
-      <c r="M8" s="1">
-        <v>62.0</v>
-      </c>
       <c r="T8" s="2"/>
       <c r="V8" s="2"/>
       <c r="W8" s="1">
-        <v>11.8</v>
+        <v>10.8</v>
       </c>
     </row>
     <row r="9">
@@ -4776,13 +4755,10 @@
       <c r="L9" s="1">
         <v>53.0</v>
       </c>
-      <c r="M9" s="1">
-        <v>52.0</v>
-      </c>
       <c r="T9" s="2"/>
       <c r="V9" s="2"/>
       <c r="W9" s="1">
-        <v>25.4</v>
+        <v>25.3</v>
       </c>
     </row>
     <row r="10">
@@ -4822,13 +4798,10 @@
       <c r="L10" s="1">
         <v>77.0</v>
       </c>
-      <c r="M10" s="1">
-        <v>95.0</v>
-      </c>
       <c r="T10" s="2"/>
       <c r="V10" s="2"/>
       <c r="W10" s="1">
-        <v>28.6</v>
+        <v>28.4</v>
       </c>
     </row>
     <row r="11">
@@ -4867,9 +4840,6 @@
       </c>
       <c r="L11" s="1">
         <v>19.0</v>
-      </c>
-      <c r="M11" s="1">
-        <v>9.0</v>
       </c>
       <c r="T11" s="2"/>
       <c r="V11" s="2"/>

</xml_diff>

<commit_message>
Switched from scipi to mip
</commit_message>
<xml_diff>
--- a/sv/data/test.xlsx
+++ b/sv/data/test.xlsx
@@ -539,7 +539,7 @@
       </c>
       <c r="S2" s="2"/>
       <c r="W2" s="1">
-        <v>6.9</v>
+        <v>7.4</v>
       </c>
     </row>
     <row r="3">
@@ -584,7 +584,7 @@
       </c>
       <c r="S3" s="2"/>
       <c r="W3" s="1">
-        <v>21.9</v>
+        <v>22.0</v>
       </c>
     </row>
     <row r="4">
@@ -629,7 +629,7 @@
       </c>
       <c r="S4" s="2"/>
       <c r="W4" s="1">
-        <v>9.8</v>
+        <v>9.7</v>
       </c>
     </row>
     <row r="5">
@@ -674,7 +674,7 @@
       </c>
       <c r="S5" s="2"/>
       <c r="W5" s="1">
-        <v>11.4</v>
+        <v>11.9</v>
       </c>
     </row>
     <row r="6">
@@ -719,7 +719,7 @@
       </c>
       <c r="S6" s="2"/>
       <c r="W6" s="1">
-        <v>18.8</v>
+        <v>19.1</v>
       </c>
     </row>
     <row r="7">
@@ -854,7 +854,7 @@
       </c>
       <c r="S9" s="2"/>
       <c r="W9" s="1">
-        <v>8.6</v>
+        <v>9.1</v>
       </c>
     </row>
     <row r="10">
@@ -899,7 +899,7 @@
       </c>
       <c r="S10" s="2"/>
       <c r="W10" s="1">
-        <v>12.9</v>
+        <v>13.9</v>
       </c>
     </row>
     <row r="11">
@@ -944,7 +944,7 @@
       </c>
       <c r="S11" s="2"/>
       <c r="W11" s="1">
-        <v>24.7</v>
+        <v>25.0</v>
       </c>
     </row>
     <row r="12">
@@ -1034,7 +1034,7 @@
       </c>
       <c r="S13" s="2"/>
       <c r="W13" s="1">
-        <v>28.1</v>
+        <v>28.3</v>
       </c>
     </row>
     <row r="14">
@@ -1169,7 +1169,7 @@
       </c>
       <c r="S16" s="2"/>
       <c r="W16" s="1">
-        <v>8.0</v>
+        <v>9.0</v>
       </c>
     </row>
     <row r="17">
@@ -1214,7 +1214,7 @@
       </c>
       <c r="S17" s="2"/>
       <c r="W17" s="1">
-        <v>8.6</v>
+        <v>8.5</v>
       </c>
     </row>
     <row r="18">
@@ -1259,7 +1259,7 @@
       </c>
       <c r="S18" s="2"/>
       <c r="W18" s="1">
-        <v>17.4</v>
+        <v>17.5</v>
       </c>
     </row>
     <row r="19">
@@ -1304,7 +1304,7 @@
       </c>
       <c r="S19" s="2"/>
       <c r="W19" s="1">
-        <v>19.3</v>
+        <v>20.3</v>
       </c>
     </row>
     <row r="20">
@@ -4454,6 +4454,9 @@
       <c r="L2" s="1">
         <v>0.0</v>
       </c>
+      <c r="M2" s="1">
+        <v>6.0</v>
+      </c>
       <c r="T2" s="2"/>
       <c r="V2" s="2"/>
       <c r="W2" s="1">
@@ -4497,6 +4500,9 @@
       <c r="L3" s="1">
         <v>5.0</v>
       </c>
+      <c r="M3" s="1">
+        <v>8.0</v>
+      </c>
       <c r="T3" s="2"/>
       <c r="V3" s="2"/>
       <c r="W3" s="1">
@@ -4540,10 +4546,13 @@
       <c r="L4" s="1">
         <v>-16.0</v>
       </c>
+      <c r="M4" s="1">
+        <v>-35.0</v>
+      </c>
       <c r="T4" s="2"/>
       <c r="V4" s="2"/>
       <c r="W4" s="1">
-        <v>10.4</v>
+        <v>10.3</v>
       </c>
     </row>
     <row r="5">
@@ -4583,10 +4592,13 @@
       <c r="L5" s="1">
         <v>22.0</v>
       </c>
+      <c r="M5" s="1">
+        <v>21.0</v>
+      </c>
       <c r="T5" s="2"/>
       <c r="V5" s="2"/>
       <c r="W5" s="1">
-        <v>9.0</v>
+        <v>9.5</v>
       </c>
     </row>
     <row r="6">
@@ -4626,10 +4638,13 @@
       <c r="L6" s="1">
         <v>25.0</v>
       </c>
+      <c r="M6" s="1">
+        <v>32.0</v>
+      </c>
       <c r="T6" s="2"/>
       <c r="V6" s="2"/>
       <c r="W6" s="1">
-        <v>29.9</v>
+        <v>23.0</v>
       </c>
     </row>
     <row r="7">
@@ -4668,6 +4683,9 @@
       </c>
       <c r="L7" s="1">
         <v>-18.0</v>
+      </c>
+      <c r="M7" s="1">
+        <v>10.0</v>
       </c>
       <c r="T7" s="2"/>
       <c r="V7" s="2"/>
@@ -4712,10 +4730,13 @@
       <c r="L8" s="1">
         <v>68.0</v>
       </c>
+      <c r="M8" s="1">
+        <v>62.0</v>
+      </c>
       <c r="T8" s="2"/>
       <c r="V8" s="2"/>
       <c r="W8" s="1">
-        <v>10.8</v>
+        <v>11.8</v>
       </c>
     </row>
     <row r="9">
@@ -4755,10 +4776,13 @@
       <c r="L9" s="1">
         <v>53.0</v>
       </c>
+      <c r="M9" s="1">
+        <v>52.0</v>
+      </c>
       <c r="T9" s="2"/>
       <c r="V9" s="2"/>
       <c r="W9" s="1">
-        <v>25.3</v>
+        <v>25.4</v>
       </c>
     </row>
     <row r="10">
@@ -4798,10 +4822,13 @@
       <c r="L10" s="1">
         <v>77.0</v>
       </c>
+      <c r="M10" s="1">
+        <v>95.0</v>
+      </c>
       <c r="T10" s="2"/>
       <c r="V10" s="2"/>
       <c r="W10" s="1">
-        <v>28.4</v>
+        <v>28.6</v>
       </c>
     </row>
     <row r="11">
@@ -4840,6 +4867,9 @@
       </c>
       <c r="L11" s="1">
         <v>19.0</v>
+      </c>
+      <c r="M11" s="1">
+        <v>9.0</v>
       </c>
       <c r="T11" s="2"/>
       <c r="V11" s="2"/>

</xml_diff>